<commit_message>
fix bug and generator
</commit_message>
<xml_diff>
--- a/sqlapp-command/src/test/resources/com/sqlapp/data/db/command/generator/TAB1.xlsx
+++ b/sqlapp-command/src/test/resources/com/sqlapp/data/db/command/generator/TAB1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satot\git\sqlapp\sqlapp-command\src\test\resources\com\sqlapp\data\db\command\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92FAB52-3B95-4231-9139-D975BFDC2729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA2629D-3B83-41D9-A0C4-D52B3D31D789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9996" yWindow="2808" windowWidth="26076" windowHeight="18480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16416" yWindow="2832" windowWidth="25068" windowHeight="17916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,53 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="游ゴシック"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Available Variables
+====
+Start Value : _start.[Column Name]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="8"/>
+            <rFont val="游ゴシック"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Available Variables
+====
+_index
+Start Value : _start.[Column Name]
+Max Value : _max.[Column Name]
+Previous Value : _previous.[Column Name]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="70">
   <si>
     <t>Table Name</t>
   </si>
@@ -30,7 +75,7 @@
     <t>TAB1</t>
   </si>
   <si>
-    <t>Number of rows</t>
+    <t>Number of Rows</t>
   </si>
   <si>
     <t>Column Name</t>
@@ -75,6 +120,24 @@
     <t>VARCHAR_COL</t>
   </si>
   <si>
+    <t>INTEGER_VALUES_COL</t>
+  </si>
+  <si>
+    <t>NUMERIC_VALUES_COL</t>
+  </si>
+  <si>
+    <t>DOUBLE_VALUES_COL</t>
+  </si>
+  <si>
+    <t>VARCHAR_VALUES_COL</t>
+  </si>
+  <si>
+    <t>INTEGER_GROUP_COL</t>
+  </si>
+  <si>
+    <t>VARCHAR_GROUP_COL</t>
+  </si>
+  <si>
     <t>Data Type</t>
   </si>
   <si>
@@ -147,52 +210,82 @@
     <t>nextAlphaNumeric( 15 )</t>
   </si>
   <si>
+    <t>nextAlphaNumeric( 20 )</t>
+  </si>
+  <si>
+    <t>addMonths(_start.DATE_COL,1)</t>
+  </si>
+  <si>
+    <t>addMonths(_start.TIMESTAMP_COL,1)</t>
+  </si>
+  <si>
+    <t>Next Value</t>
+  </si>
+  <si>
+    <t>addSeconds(_previous.TIME_COL,1)</t>
+  </si>
+  <si>
+    <t>addMilliSeconds(_previous.TIMESTAMP_COL,1)</t>
+  </si>
+  <si>
+    <t>_previous.TINYINT_COL + 1</t>
+  </si>
+  <si>
+    <t>_previous.SMALLINT_COL + 1</t>
+  </si>
+  <si>
+    <t>_previous.INTEGER_COL + 1</t>
+  </si>
+  <si>
+    <t>_previous.BIGINT_COL + 1</t>
+  </si>
+  <si>
+    <t>_previous.NUMERIC_COL + 1</t>
+  </si>
+  <si>
+    <t>nextDouble(0.0d, 1000.0d)</t>
+  </si>
+  <si>
+    <t>!_previous.BOOLEAN_COL</t>
+  </si>
+  <si>
+    <t>_previous.INTEGER_VALUES_COL + 1</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>SELECT　SQL</t>
+  </si>
+  <si>
+    <t>abc</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>ghi</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>Group1</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>SELECT 1 AS INTEGER_GROUP_COL, 'XXX' AS VARCHAR_GROUP_COL  FROM (VALUES(0))
+UNION ALL
+SELECT 1 AS INTEGER_GROUP_COL, 'XXX' AS VARCHAR_GROUP_COL  FROM (VALUES(0))</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
     <t>Max Value</t>
-  </si>
-  <si>
-    <t>LocalDate.of(2025,4,1)</t>
-  </si>
-  <si>
-    <t>LocalDateTime.of(2025,4,1,0,0,0)</t>
-  </si>
-  <si>
-    <t>Next Value</t>
-  </si>
-  <si>
-    <t>addDays(_previous.DATE_COL, 1)</t>
-  </si>
-  <si>
-    <t>addSeconds(_previous.TIME_COL, 1)</t>
-  </si>
-  <si>
-    <t>addMilliSeconds(_previous.TIMESTAMP_COL, 1)</t>
-  </si>
-  <si>
-    <t>_previous.TINYINT_COL + 1</t>
-  </si>
-  <si>
-    <t>_previous.SMALLINT_COL + 1</t>
-  </si>
-  <si>
-    <t>_previous.INTEGER_COL + 1</t>
-  </si>
-  <si>
-    <t>_previous.BIGINT_COL + 1</t>
-  </si>
-  <si>
-    <t>_previous.NUMERIC_COL + 1</t>
-  </si>
-  <si>
-    <t>nextDouble(0.0d, 1000.0d)</t>
-  </si>
-  <si>
-    <t>!_previous.BOOLEAN_COL</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>SELECT　SQL</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>addDays(_previous.DATE_COL,1)</t>
+    <phoneticPr fontId="20"/>
   </si>
 </sst>
 </file>
@@ -303,16 +396,17 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <vertAlign val="superscript"/>
-      <sz val="16"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,7 +451,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -397,28 +491,34 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -737,13 +837,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.4">
@@ -763,34 +863,45 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="32.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="29.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.09765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.8984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.19921875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -833,98 +944,152 @@
       <c r="N1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="O1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="N2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
       <c r="A4" s="9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10" t="b">
         <v>0</v>
@@ -965,19 +1130,37 @@
       <c r="N4" s="10" t="b">
         <v>0</v>
       </c>
+      <c r="O4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" s="10" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E5" s="12">
         <v>1</v>
@@ -995,148 +1178,221 @@
         <v>1</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>40</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="O5" s="12">
+        <v>1</v>
+      </c>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
     </row>
-    <row r="6" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="14">
+    <row r="6" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A6" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="13">
         <v>127</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>32767</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>2147483647</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>9.2233720368547758E+18</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <v>100</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>1.7976931348623157E+308</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>1.7976931348623157E+308</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13">
+        <v>2147483647</v>
+      </c>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
     </row>
-    <row r="7" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A7" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="16" t="s">
+    <row r="7" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="M7" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="N7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="O7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="16" t="s">
-        <v>40</v>
-      </c>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="1:14" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A8" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
+    <row r="8" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17">
+        <v>1000.123</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>1.17</v>
+      </c>
+      <c r="R8" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+    </row>
+    <row r="9" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="D9" s="20"/>
+      <c r="P9" s="20">
+        <v>1111.2339999999999</v>
+      </c>
+      <c r="Q9">
+        <v>1.18</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="P10" s="20">
+        <v>2222.3449999999998</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>1.19</v>
+      </c>
+      <c r="R10" s="20" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
-        <v>30</v>
+    <row r="1" spans="1:2" ht="23.4" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="23.4" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
-        <v>56</v>
+    <row r="2" spans="1:2" ht="90" x14ac:dyDescent="0.4">
+      <c r="A2" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>